<commit_message>
Added DS 775 Wk 10 and Wk 11
</commit_message>
<xml_diff>
--- a/wk8/HW_8_Isaacson.xlsx
+++ b/wk8/HW_8_Isaacson.xlsx
@@ -18,14 +18,28 @@
     <sheet name="Problem5" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="LSGRGeng_RelaxBounds" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="3" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="3" hidden="1">FALSE</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="3" hidden="1">TRUE</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Problem1!$C$7:$D$7</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Problem2!$B$7:$C$7</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Problem4!$C$6</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">Problem5!$D$9:$F$9</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Problem5!$D$11:$F$11</definedName>
+    <definedName name="solver_adj_ob" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_cha" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_chc1" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_chn" localSheetId="3" hidden="1">4</definedName>
+    <definedName name="solver_chp1" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_cht" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_cir1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_con" localSheetId="3" hidden="1">" "</definedName>
+    <definedName name="solver_con1" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_dia" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
@@ -38,16 +52,26 @@
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_iao" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_int" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_irs" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ism" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_kiv" localSheetId="3" hidden="1">2E+30</definedName>
+    <definedName name="solver_lhs_ob1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Problem1!$C$9</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Problem2!$B$10</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">Problem4!$C$6</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Problem5!$F$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Problem5!$F$11</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Problem2!$B$11</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">Problem4!$C$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Problem5!$G$7:$G$9</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_lva" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_mda" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
@@ -56,6 +80,7 @@
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mod" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
@@ -72,38 +97,49 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_ntr" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ntri" hidden="1">1000</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_obc" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_obp" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Problem1!$G$7</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Problem2!$F$7</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">Problem4!$H$6</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Problem5!$I$9</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Problem5!$I$11</definedName>
+    <definedName name="solver_opt_ob" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_psi" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rdp" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_reco1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rep" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Problem1!$E$9</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">Problem2!$D$10</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">Problem4!$D$8</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Problem5!$F$12</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Problem5!$F$14</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Problem2!$D$11</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">Problem4!$C$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Problem5!$I$7:$I$9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
@@ -112,14 +148,24 @@
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsmp" hidden="1">2</definedName>
+    <definedName name="solver_rtr" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rxc1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rxv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_seed" hidden="1">0</definedName>
+    <definedName name="solver_sel" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_slv" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_slvu" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_spid" localSheetId="3" hidden="1">" "</definedName>
+    <definedName name="solver_srvr" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
@@ -128,6 +174,7 @@
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tms" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
@@ -136,14 +183,21 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_umod" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_urs" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_userid" localSheetId="3" hidden="1">319624</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_var" localSheetId="3" hidden="1">" "</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_vir" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_vol" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_vst" localSheetId="3" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -155,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Problem 1</t>
   </si>
@@ -597,20 +651,20 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.3984375" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" s="2">
         <v>8</v>
       </c>
@@ -624,7 +678,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>1.9999999880790711</v>
       </c>
@@ -636,7 +690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C9">
         <f>C7+D7</f>
         <v>2</v>
@@ -661,18 +715,18 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>4</v>
       </c>
@@ -683,7 +737,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>2.200000199999999</v>
       </c>
@@ -695,7 +749,7 @@
         <v>27.759997720000975</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10" s="2">
         <f>20*B7+30*C7</f>
         <v>50.00000099999999</v>
@@ -707,7 +761,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="2">
         <f>5*B7+10*C7</f>
         <v>13</v>
@@ -732,19 +786,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" s="2">
         <v>100</v>
       </c>
@@ -764,7 +818,7 @@
         <v>-5095</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="3">
         <v>3.1838893257032788</v>
       </c>
@@ -774,7 +828,7 @@
         <v>906.90190542387245</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -782,7 +836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>0</v>
       </c>
@@ -797,20 +851,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.265625" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -824,7 +878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="D2">
         <v>100</v>
       </c>
@@ -835,106 +889,164 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D3">
+        <f>(-1/3+3/3)</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="E3">
+        <f>(-1/4+4/4)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F3">
+        <f>(-1/2+2/2)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <f>D1*D11+D2*D11^D3</f>
+        <v>1940.3054175455327</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:F4" si="0">E1*E11+E2*E11^E3</f>
+        <v>1545.6699506378895</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>556.41946035530952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D5">
         <v>-25</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>-10</v>
       </c>
-      <c r="F3">
+      <c r="F5">
         <v>-15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D7" s="2">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="G7">
+        <f>SUMPRODUCT(D7:F7,$D$11:$F$11)</f>
+        <v>500.00000269546035</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="G8">
+        <f t="shared" ref="G8:G9" si="1">SUMPRODUCT(D8:F8,$D$11:$F$11)</f>
+        <v>350.00000198518592</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.65714278740536614</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.31428578938762752</v>
-      </c>
-      <c r="G9" t="e">
-        <f>(D1+D2*D9^(-1/3))+(E1+E2*E9^(-1/4))+(F1+F2*F9^(-1/2))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9">
-        <f>+D3*D9+E3*E9+F3*F9</f>
-        <v>-11.285714714868075</v>
-      </c>
-      <c r="I9" s="5" t="e">
-        <f>+G9+H9</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>120.80485050240516</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D11" s="3">
+        <v>28.672055577529775</v>
+      </c>
+      <c r="E11" s="3">
+        <v>51.659931024384264</v>
+      </c>
+      <c r="F11" s="3">
+        <v>17.394341884907917</v>
+      </c>
+      <c r="G11">
+        <f>D4+E4+F4</f>
+        <v>4042.3948285387319</v>
+      </c>
+      <c r="H11">
+        <f>+D5*D11+E5*E11+F5*F11</f>
+        <v>-1494.315827955706</v>
+      </c>
+      <c r="I11" s="5">
+        <f>+G11+H11</f>
+        <v>2548.0790005830258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>1</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <v>20</v>
       </c>
     </row>

</xml_diff>